<commit_message>
Riferimenti caption Tabelle e Figure
</commit_message>
<xml_diff>
--- a/Relazione_tabella_comparativa.xlsx
+++ b/Relazione_tabella_comparativa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unipiit-my.sharepoint.com/personal/a_camici1_studenti_unipi_it/Documents/Appunti università/M/Linguistica computazionale 2/GxG_Camici/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="172" documentId="11_AD4D5CB4E552A5DACE1C641400DF5AC45BDEDD8B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2CC6634-50A0-45F7-8DD5-9357E5939406}"/>
+  <xr:revisionPtr revIDLastSave="188" documentId="11_AD4D5CB4E552A5DACE1C641400DF5AC45BDEDD8B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1BF790EF-BD79-4A55-A25F-2FC51CA49759}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="63">
   <si>
     <t>accuracy</t>
   </si>
@@ -219,14 +219,46 @@
     <t>[[53, 47], [52, 48]]</t>
   </si>
   <si>
-    <t>Tabella XXXX: Metriche di valutazione del modello SVM con ProfilingUD sui dati di test suddivisi per genere</t>
+    <r>
+      <t xml:space="preserve">Tabella REPORT5FOLD: Report della </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>5 fold cross</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> validation del mo-dello SVM con ProfilingUD </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Report finale sul test set di SVM ProfilingUD </t>
+  </si>
+  <si>
+    <t>0.5729</t>
+  </si>
+  <si>
+    <t>0.57</t>
+  </si>
+  <si>
+    <t>[[69, 31], [54, 45]]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,8 +358,14 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -343,12 +381,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -435,7 +467,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -449,6 +481,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -458,61 +514,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -809,10 +838,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -827,19 +856,21 @@
     <col min="9" max="9" width="17.46484375" style="1" customWidth="1"/>
     <col min="10" max="10" width="9.06640625" style="1"/>
     <col min="11" max="11" width="15.53125" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.06640625" style="1"/>
+    <col min="12" max="16" width="9.06640625" style="1"/>
+    <col min="17" max="17" width="14.86328125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-    </row>
-    <row r="2" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+    </row>
+    <row r="2" spans="1:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -859,8 +890,15 @@
       <c r="I2" s="17"/>
       <c r="J2" s="17"/>
       <c r="K2" s="18"/>
-    </row>
-    <row r="3" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="M2" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="18"/>
+    </row>
+    <row r="3" spans="1:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -889,8 +927,21 @@
       <c r="K3" s="20" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="M3" s="19"/>
+      <c r="N3" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="O3" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="P3" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -921,8 +972,23 @@
       <c r="K4" s="22" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="M4" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="N4" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="O4" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="P4" s="22">
+        <v>199</v>
+      </c>
+      <c r="Q4" s="22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -945,8 +1011,15 @@
       <c r="I5" s="24"/>
       <c r="J5" s="22"/>
       <c r="K5" s="22"/>
-    </row>
-    <row r="6" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="M5" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="N5" s="24"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="22"/>
+    </row>
+    <row r="6" spans="1:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -969,8 +1042,15 @@
       <c r="I6" s="22"/>
       <c r="J6" s="22"/>
       <c r="K6" s="22"/>
-    </row>
-    <row r="7" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="M6" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="N6" s="22"/>
+      <c r="O6" s="22"/>
+      <c r="P6" s="22"/>
+      <c r="Q6" s="22"/>
+    </row>
+    <row r="7" spans="1:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G7" s="23" t="s">
         <v>53</v>
       </c>
@@ -978,25 +1058,39 @@
       <c r="I7" s="24"/>
       <c r="J7" s="22"/>
       <c r="K7" s="22"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="G8" s="14" t="s">
+      <c r="M7" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="N7" s="24"/>
+      <c r="O7" s="24"/>
+      <c r="P7" s="22"/>
+      <c r="Q7" s="22"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="G8" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A9" s="6" t="s">
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="M8" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="25"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A9" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>36</v>
       </c>
@@ -1010,7 +1104,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -1024,7 +1118,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>2</v>
       </c>
@@ -1037,13 +1131,11 @@
       <c r="D12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>3</v>
       </c>
@@ -1056,12 +1148,12 @@
       <c r="D13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>4</v>
       </c>
@@ -1074,12 +1166,12 @@
       <c r="D14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>5</v>
       </c>
@@ -1092,30 +1184,28 @@
       <c r="D15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="9"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="D16" s="8"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="K16" s="25"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="K16" s="9"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
@@ -1127,11 +1217,10 @@
       <c r="C18" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
@@ -1143,11 +1232,10 @@
       <c r="C19" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
@@ -1159,16 +1247,15 @@
       <c r="C20" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
@@ -1180,12 +1267,10 @@
       <c r="C21" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="8"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
@@ -1197,12 +1282,6 @@
       <c r="C22" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
@@ -1214,34 +1293,17 @@
       <c r="C23" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
     <mergeCell ref="G2:K2"/>
     <mergeCell ref="G8:K8"/>
     <mergeCell ref="I20:M20"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A9:D9"/>
     <mergeCell ref="A17:C17"/>
+    <mergeCell ref="M2:Q2"/>
+    <mergeCell ref="M8:Q8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Ngrams, relazione e notebook children
</commit_message>
<xml_diff>
--- a/Relazione_tabella_comparativa.xlsx
+++ b/Relazione_tabella_comparativa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unipiit-my.sharepoint.com/personal/a_camici1_studenti_unipi_it/Documents/Appunti università/M/Linguistica computazionale 2/GxG_Camici/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="188" documentId="11_AD4D5CB4E552A5DACE1C641400DF5AC45BDEDD8B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1BF790EF-BD79-4A55-A25F-2FC51CA49759}"/>
+  <xr:revisionPtr revIDLastSave="305" documentId="11_AD4D5CB4E552A5DACE1C641400DF5AC45BDEDD8B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DAC6FF26-42EE-4B9B-966D-382055AC1F3C}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="77">
   <si>
     <t>accuracy</t>
   </si>
@@ -253,12 +253,54 @@
   <si>
     <t>[[69, 31], [54, 45]]</t>
   </si>
+  <si>
+    <t>mean accuracy</t>
+  </si>
+  <si>
+    <t>tipo</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>POS</t>
+  </si>
+  <si>
+    <t>lemma</t>
+  </si>
+  <si>
+    <t>char</t>
+  </si>
+  <si>
+    <t>0.58</t>
+  </si>
+  <si>
+    <t>0.54</t>
+  </si>
+  <si>
+    <t>0.55</t>
+  </si>
+  <si>
+    <t>0.52</t>
+  </si>
+  <si>
+    <t>0.49</t>
+  </si>
+  <si>
+    <t>0.46</t>
+  </si>
+  <si>
+    <t>word</t>
+  </si>
+  <si>
+    <t>[[48, 52], [52, 47]]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -364,6 +406,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="STXinwei"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -467,82 +515,121 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -838,467 +925,818 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q23"/>
+  <dimension ref="A1:AH35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:Q8"/>
+    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AB1" sqref="AB1:AH6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.06640625" style="1"/>
-    <col min="2" max="2" width="11.19921875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.1328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.06640625" style="1"/>
-    <col min="5" max="5" width="16.6640625" style="1" customWidth="1"/>
-    <col min="6" max="7" width="9.06640625" style="1"/>
-    <col min="8" max="8" width="12.3984375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.46484375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.06640625" style="1"/>
-    <col min="11" max="11" width="15.53125" style="1" customWidth="1"/>
-    <col min="12" max="16" width="9.06640625" style="1"/>
-    <col min="17" max="17" width="14.86328125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.06640625" style="1"/>
+    <col min="1" max="1" width="9.06640625" style="2"/>
+    <col min="2" max="2" width="11.19921875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.1328125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.06640625" style="2"/>
+    <col min="5" max="5" width="16.6640625" style="2" customWidth="1"/>
+    <col min="6" max="7" width="9.06640625" style="2"/>
+    <col min="8" max="8" width="12.3984375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="17.46484375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9.06640625" style="2"/>
+    <col min="11" max="11" width="15.53125" style="2" customWidth="1"/>
+    <col min="12" max="16" width="9.06640625" style="2"/>
+    <col min="17" max="17" width="14.86328125" style="2" customWidth="1"/>
+    <col min="18" max="23" width="9.06640625" style="2"/>
+    <col min="24" max="24" width="14.53125" style="2" customWidth="1"/>
+    <col min="25" max="28" width="9.06640625" style="2"/>
+    <col min="29" max="29" width="4.86328125" style="2" customWidth="1"/>
+    <col min="30" max="30" width="3" style="2" customWidth="1"/>
+    <col min="31" max="31" width="8.06640625" style="2" customWidth="1"/>
+    <col min="32" max="32" width="12.19921875" style="2" customWidth="1"/>
+    <col min="33" max="33" width="9.9296875" style="2" customWidth="1"/>
+    <col min="34" max="16384" width="9.06640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:34" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-    </row>
-    <row r="2" spans="1:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="3" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="V1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC1" s="3"/>
+      <c r="AD1" s="3"/>
+      <c r="AE1" s="3"/>
+      <c r="AF1" s="3"/>
+      <c r="AG1" s="3"/>
+      <c r="AH1" s="3"/>
+    </row>
+    <row r="2" spans="1:34" ht="26.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="18"/>
-      <c r="M2" s="16" t="s">
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="7"/>
+      <c r="M2" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="18"/>
-    </row>
-    <row r="3" spans="1:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="4" t="s">
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="7"/>
+      <c r="V2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="W2" s="2">
+        <v>3</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB2" s="13"/>
+      <c r="AC2" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD2" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF2" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" ht="39.75" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="2">
         <v>199</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="19"/>
-      <c r="H3" s="20" t="s">
+      <c r="G3" s="10"/>
+      <c r="H3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="20" t="s">
+      <c r="I3" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="J3" s="20" t="s">
+      <c r="J3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="K3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="19"/>
-      <c r="N3" s="20" t="s">
+      <c r="M3" s="10"/>
+      <c r="N3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="O3" s="20" t="s">
+      <c r="O3" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="P3" s="20" t="s">
+      <c r="P3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="Q3" s="20" t="s">
+      <c r="Q3" s="11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="2" t="s">
+      <c r="V3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="W3" s="2">
+        <v>1</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB3" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC3" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD3" s="13">
+        <v>3</v>
+      </c>
+      <c r="AE3" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF3" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="AG3" s="13">
+        <v>199</v>
+      </c>
+      <c r="AH3" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="2">
         <v>74</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="G4" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="H4" s="22" t="s">
+      <c r="H4" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="I4" s="22" t="s">
+      <c r="I4" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="J4" s="22">
+      <c r="J4" s="16">
         <v>200</v>
       </c>
-      <c r="K4" s="22" t="s">
+      <c r="K4" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="M4" s="21" t="s">
+      <c r="M4" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="N4" s="22" t="s">
+      <c r="N4" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="O4" s="22" t="s">
+      <c r="O4" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="P4" s="22">
+      <c r="P4" s="16">
         <v>199</v>
       </c>
-      <c r="Q4" s="22" t="s">
+      <c r="Q4" s="16" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="2" t="s">
+      <c r="V4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="W4" s="2">
+        <v>2</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB4" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC4" s="17"/>
+      <c r="AD4" s="12"/>
+      <c r="AE4" s="12"/>
+      <c r="AF4" s="13"/>
+      <c r="AG4" s="13"/>
+    </row>
+    <row r="5" spans="1:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A5" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="2">
         <v>200</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="23" t="s">
+      <c r="G5" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="22"/>
-      <c r="M5" s="23" t="s">
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="M5" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="N5" s="24"/>
-      <c r="O5" s="24"/>
-      <c r="P5" s="22"/>
-      <c r="Q5" s="22"/>
-    </row>
-    <row r="6" spans="1:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="2" t="s">
+      <c r="N5" s="19"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+      <c r="V5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="W5" s="2">
+        <v>3</v>
+      </c>
+      <c r="X5" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB5" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC5" s="17"/>
+      <c r="AD5" s="13"/>
+      <c r="AE5" s="13"/>
+      <c r="AF5" s="13"/>
+      <c r="AG5" s="13"/>
+    </row>
+    <row r="6" spans="1:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A6" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="2">
         <v>152</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="G6" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
-      <c r="M6" s="23" t="s">
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="M6" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="N6" s="22"/>
-      <c r="O6" s="22"/>
-      <c r="P6" s="22"/>
-      <c r="Q6" s="22"/>
-    </row>
-    <row r="7" spans="1:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="G7" s="23" t="s">
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="V6" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="W6" s="2">
+        <v>3</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB6" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-      <c r="M7" s="23" t="s">
+      <c r="AC6" s="17"/>
+      <c r="AD6" s="12"/>
+      <c r="AE6" s="12"/>
+      <c r="AF6" s="13"/>
+      <c r="AG6" s="13"/>
+    </row>
+    <row r="7" spans="1:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G7" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="N7" s="24"/>
-      <c r="O7" s="24"/>
-      <c r="P7" s="22"/>
-      <c r="Q7" s="22"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="G8" s="11" t="s">
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="M7" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="N7" s="19"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16"/>
+      <c r="V7" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="W7" s="2">
+        <v>1</v>
+      </c>
+      <c r="X7" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="G8" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="M8" s="25" t="s">
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="M8" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="N8" s="25"/>
-      <c r="O8" s="25"/>
-      <c r="P8" s="25"/>
-      <c r="Q8" s="25"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A9" s="14" t="s">
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="21"/>
+      <c r="V8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="W8" s="2">
+        <v>3</v>
+      </c>
+      <c r="X8" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="A9" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A10" s="3" t="s">
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="V9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="W9" s="2">
+        <v>1</v>
+      </c>
+      <c r="X9" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="A10" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A11" s="1">
+      <c r="V10" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="W10" s="2">
         <v>1</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="X10" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="A11" s="2">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A12" s="1">
+      <c r="V11" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="W11" s="2">
         <v>2</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="X11" s="24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="A12" s="2">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A13" s="1">
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="V12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="W12" s="2">
         <v>3</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="X12" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="A13" s="2">
+        <v>3</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A14" s="1">
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+      <c r="V13" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="W13" s="2">
+        <v>2</v>
+      </c>
+      <c r="X13" s="2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="A14" s="2">
         <v>4</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A15" s="1">
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="A15" s="2">
         <v>5</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="5"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="K16" s="9"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="35"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="36"/>
+      <c r="K17" s="36"/>
+      <c r="L17" s="37"/>
+      <c r="M17" s="37"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="36"/>
+      <c r="K18" s="36"/>
+      <c r="L18" s="37"/>
+      <c r="M18" s="37"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A19" s="1">
+      <c r="A19" s="2">
         <v>1</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="36"/>
+      <c r="K19" s="36"/>
+      <c r="L19" s="37"/>
+      <c r="M19" s="37"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A20" s="1">
+      <c r="A20" s="2">
         <v>2</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="12"/>
-      <c r="L20" s="12"/>
-      <c r="M20" s="12"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
+      <c r="K20" s="36"/>
+      <c r="L20" s="38"/>
+      <c r="M20" s="38"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A21" s="1">
+      <c r="A21" s="2">
         <v>3</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="36"/>
+      <c r="L21" s="37"/>
+      <c r="M21" s="37"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A22" s="1">
+      <c r="A22" s="2">
         <v>4</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="2" t="s">
         <v>48</v>
       </c>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="36"/>
+      <c r="K22" s="36"/>
+      <c r="L22" s="37"/>
+      <c r="M22" s="37"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A23" s="1">
+      <c r="A23" s="2">
         <v>5</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="36"/>
+      <c r="K23" s="36"/>
+      <c r="L23" s="37"/>
+      <c r="M23" s="37"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="G24" s="36"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="36"/>
+      <c r="K24" s="36"/>
+      <c r="L24" s="37"/>
+      <c r="M24" s="37"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="G25" s="36"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="36"/>
+      <c r="J25" s="36"/>
+      <c r="K25" s="36"/>
+      <c r="L25" s="37"/>
+      <c r="M25" s="37"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="G26" s="36"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="36"/>
+      <c r="K26" s="36"/>
+      <c r="L26" s="37"/>
+      <c r="M26" s="37"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
+      <c r="K27" s="36"/>
+      <c r="L27" s="37"/>
+      <c r="M27" s="37"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="G28" s="36"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="36"/>
+      <c r="K28" s="36"/>
+      <c r="L28" s="37"/>
+      <c r="M28" s="37"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="G29" s="36"/>
+      <c r="H29" s="36"/>
+      <c r="I29" s="36"/>
+      <c r="J29" s="36"/>
+      <c r="K29" s="36"/>
+      <c r="L29" s="37"/>
+      <c r="M29" s="37"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="G30" s="36"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="36"/>
+      <c r="J30" s="36"/>
+      <c r="K30" s="36"/>
+      <c r="L30" s="37"/>
+      <c r="M30" s="37"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="G31" s="37"/>
+      <c r="H31" s="37"/>
+      <c r="I31" s="37"/>
+      <c r="J31" s="37"/>
+      <c r="K31" s="37"/>
+      <c r="L31" s="37"/>
+      <c r="M31" s="37"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="G32" s="37"/>
+      <c r="H32" s="37"/>
+      <c r="I32" s="37"/>
+      <c r="J32" s="37"/>
+      <c r="K32" s="37"/>
+      <c r="L32" s="37"/>
+      <c r="M32" s="37"/>
+    </row>
+    <row r="33" spans="7:13" x14ac:dyDescent="0.45">
+      <c r="G33" s="37"/>
+      <c r="H33" s="37"/>
+      <c r="I33" s="37"/>
+      <c r="J33" s="37"/>
+      <c r="K33" s="37"/>
+      <c r="L33" s="37"/>
+      <c r="M33" s="37"/>
+    </row>
+    <row r="34" spans="7:13" x14ac:dyDescent="0.45">
+      <c r="G34" s="37"/>
+      <c r="H34" s="37"/>
+      <c r="I34" s="37"/>
+      <c r="J34" s="37"/>
+      <c r="K34" s="37"/>
+      <c r="L34" s="37"/>
+      <c r="M34" s="37"/>
+    </row>
+    <row r="35" spans="7:13" x14ac:dyDescent="0.45">
+      <c r="G35" s="37"/>
+      <c r="H35" s="37"/>
+      <c r="I35" s="37"/>
+      <c r="J35" s="37"/>
+      <c r="K35" s="37"/>
+      <c r="L35" s="37"/>
+      <c r="M35" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="AB1:AH1"/>
     <mergeCell ref="G2:K2"/>
     <mergeCell ref="G8:K8"/>
-    <mergeCell ref="I20:M20"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A9:D9"/>
     <mergeCell ref="A17:C17"/>

</xml_diff>